<commit_message>
updated documentation on datasets
</commit_message>
<xml_diff>
--- a/06_guide_to_datasets.xlsx
+++ b/06_guide_to_datasets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d8c41f4a4675e5d/Documents/PhD/Thesis/Quantitative strand/social_rent_rdd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meng-Le\Documents\IJHP_replication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="11_F25DC773A252ABDACC10480141D944465ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FF400C6-4C81-4864-830B-908B523D3826}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EDE6EC-89FF-48A0-B768-E7D2DE649557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1308" yWindow="-108" windowWidth="21840" windowHeight="15576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>File name</t>
   </si>
@@ -36,18 +36,12 @@
     <t>Usage</t>
   </si>
   <si>
-    <t>SDR 2015/16</t>
-  </si>
-  <si>
     <t>Affordability gap</t>
   </si>
   <si>
     <t>SDR_Data_Release_2016_v01.xlsx</t>
   </si>
   <si>
-    <t>VOA 2015/16</t>
-  </si>
-  <si>
     <t>Publication_AllTables_17112016.xlsx</t>
   </si>
   <si>
@@ -181,6 +175,27 @@
   </si>
   <si>
     <t>https://www.gov.uk/government/collections/private-registered-provider-social-housing-stock-in-england</t>
+  </si>
+  <si>
+    <t>Housing and Communities Agency (HCA) Standard Data Return (SDR) 2015/16</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Valuation Office Agency (VOA)  Private Rental Market Statistics (PRMS) 2015/16</t>
+  </si>
+  <si>
+    <t>Statistical return series detailing social rents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistical return series detailing social rents. This version was used to measure affordability pressure </t>
+  </si>
+  <si>
+    <t>Statistical return series detailing private rents</t>
+  </si>
+  <si>
+    <t>Statistical return for private rents taken over by the Office for National Statistics with VOA data</t>
   </si>
 </sst>
 </file>
@@ -508,311 +523,326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="107.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" customWidth="1"/>
-    <col min="4" max="4" width="69" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61" customWidth="1"/>
+    <col min="1" max="2" width="107.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="5" max="5" width="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44642</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44642</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44545</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>44640</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>44545</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>44642</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>44545</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2">
+        <v>44642</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2">
+        <v>44545</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>44642</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2">
+        <v>44637</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2">
+        <v>44640</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2">
+        <v>44951</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2">
+        <v>44951</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="2">
+        <v>44887</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2">
-        <v>44642</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2">
-        <v>44642</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2">
-        <v>44545</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>44640</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2">
-        <v>44545</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2">
-        <v>44642</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2">
-        <v>44545</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2">
-        <v>44642</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2">
-        <v>44545</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2">
-        <v>44642</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="2">
-        <v>44637</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="2">
-        <v>44640</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="2">
-        <v>44951</v>
-      </c>
-      <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2">
-        <v>44951</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="2">
+        <v>44967</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="2">
-        <v>44887</v>
-      </c>
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="2">
-        <v>44967</v>
-      </c>
-      <c r="D17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>